<commit_message>
working , docker tested done
</commit_message>
<xml_diff>
--- a/multi_asset.xlsx
+++ b/multi_asset.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,126 +497,126 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>1,211</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1,150</t>
+          <t>1,197</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1,220</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5,000</t>
+          <t>5,132</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4,800</t>
+          <t>4,821</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1,300</t>
+          <t>1,202</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1,180</t>
+          <t>1,373</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>1,386</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>5,100</t>
+          <t>4,980</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4,900</t>
+          <t>4,853</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>92%</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>89%</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Check AFBC-1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-400</t>
+          <t>1,155</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>1,127</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1,406</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>53</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -626,22 +626,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>5,050</t>
+          <t>4,895</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>4,950</t>
+          <t>4,927</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>105%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -653,50 +653,2369 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1,250</t>
+          <t>1,286</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1,170</t>
+          <t>1,110</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1350</t>
+          <t>1,200</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4,822</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>4,964</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>101%</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>-329</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1,497</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1,387</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>49</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>5,014</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4,893</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1,436</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1,440</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1,325</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>47</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>4,980</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>4,820</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>5,101</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>4,909</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1,426</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1,298</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1,344</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>5,138</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>5,041</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>104%</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1,298</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1,444</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1,205</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>4,965</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>4,825</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1,190</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1,104</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1,292</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>4,975</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>5,169</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1,472</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1,474</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1,211</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>4,936</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>5,041</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1,351</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1,117</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1,255</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>5,161</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>5,110</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>109%</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1,423</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1,430</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1,126</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>4,891</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5,006</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1,402</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1,346</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1,213</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>4,855</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>4,964</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1,223</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1,197</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1,497</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>5,055</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>4,997</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1,262</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1,187</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1,419</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>5,137</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>4,942</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1,370</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1,262</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1,344</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>4,872</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>5,051</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1,169</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1,483</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1,480</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>5,131</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>4,853</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>86%</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1,124</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1,473</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1,194</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>5,161</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>5,171</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>86%</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>89%</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>-105</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1,231</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1,323</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>5,017</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>5,141</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1,266</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1,326</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1,342</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>5,004</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>5,197</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1,359</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1,269</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1,275</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>5,082</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>5,176</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1,206</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1,381</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-156</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>4,863</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>5,116</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1,293</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1,255</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1,343</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>5,144</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>4,931</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>106%</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>86%</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1,429</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1,225</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1,324</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>5,166</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>4,819</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1,230</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1,216</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1,485</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>4,903</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>5,061</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1,276</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1,195</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1,220</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>4,961</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>4,943</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1,264</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1,245</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1,180</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>5,146</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>4,904</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>1,472</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>1,308</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1,460</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>5,113</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>5,111</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>1,338</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>1,227</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1,401</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4,860</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>4,976</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>1,172</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1,454</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>-276</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>4,972</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>4,988</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>1,361</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1,274</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1,409</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>5,060</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>4,858</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>1,119</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1,289</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1,295</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>4,877</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>4,832</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>1,370</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1,147</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1,244</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>5,162</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>5,099</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>102%</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>1,299</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1,292</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1,108</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>4,988</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>5,140</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>1,150</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1,163</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1,219</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>5,017</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>5,178</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>1,294</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1,384</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1,445</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>5,028</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>4,967</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>1,360</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1,148</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1,103</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>4,846</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>4,938</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>1,282</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>1,202</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1,267</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>5,125</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>5,105</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>1,470</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1,439</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1,368</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4,849</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>5,021</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>1,216</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1,222</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1,268</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>4,923</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>5,056</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>1,479</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1,484</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1,175</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>4,830</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>5,164</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>105%</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>1,205</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1,494</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1,210</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>5,184</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>4,943</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>1,160</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1,493</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>1,274</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>5,094</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>5,111</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>1,139</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1,360</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1,112</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>4,965</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>5,136</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Minor fluctuation</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>1,386</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1,319</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1,221</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>4,910</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>4,930</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>1,456</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1,317</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>-396</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>5,023</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>4,921</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>1,420</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1,272</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1,255</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>5,115</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>4,898</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>1,418</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1,321</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1,206</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>4,981</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>4,970</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>-403</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1,454</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1,116</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>5,152</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>5,096</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>86%</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>90%</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>1,363</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1,181</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1,208</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>4,852</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>5,111</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Check AFBC-1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>